<commit_message>
Fixed rare candy program (properly track hand and prize pile), added remove from deck
</commit_message>
<xml_diff>
--- a/Project 1/RareCandyStats/RareCandyBrickOutput.xlsx
+++ b/Project 1/RareCandyStats/RareCandyBrickOutput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rance\OneDrive\Documents\My Files\Other\College Class Materials\ThirdYearSpring\Probability and Applied Statistics\Projects\Project 1\RareCandyStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1398FE05-3730-4342-8E5D-6F181E12B10D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DC5F1E-5A4B-4B1A-8F12-86D34AA8A2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{0A98BBD3-9A80-4CA7-96FD-69E6A1CD7B49}"/>
   </bookViews>
@@ -242,16 +242,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>9.5000000000000001E-2</c:v>
+                  <c:v>9.8900000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.38E-2</c:v>
+                  <c:v>8.6E-3</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.3999999999999998E-3</c:v>
+                <c:pt idx="2" formatCode="0.00E+00">
+                  <c:v>8.0000000000000004E-4</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>2.9999999999999997E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1477,7 +1477,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1499,7 +1499,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>9.5000000000000001E-2</v>
+        <v>9.8900000000000002E-2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1507,15 +1507,15 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1.38E-2</v>
+        <v>8.6E-3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>2.3999999999999998E-3</v>
+      <c r="B4" s="1">
+        <v>8.0000000000000004E-4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1523,7 +1523,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>2.9999999999999997E-4</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>